<commit_message>
Sprawka z fizy i odswierzony vault
</commit_message>
<xml_diff>
--- a/Fizyka/Fizyka/Lab 2 O1/Zeszyt1.xlsx
+++ b/Fizyka/Fizyka/Lab 2 O1/Zeszyt1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedScorp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedScorp\Desktop\Sprawozdania\Fizyka\Fizyka\Lab 2 O1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98669188-BD2B-4F2D-9FE3-5E3260B5D8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7804DD-1A79-49F7-B69B-8E5A361BFE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{CB43EC45-3054-4F49-8FA5-F7570E09B84F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CB43EC45-3054-4F49-8FA5-F7570E09B84F}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Pomiary</t>
   </si>
@@ -50,12 +39,6 @@
     <t>(avg(f)-f)^2</t>
   </si>
   <si>
-    <t>Ub</t>
-  </si>
-  <si>
-    <t>Przyrządy</t>
-  </si>
-  <si>
     <t>x[cm]</t>
   </si>
   <si>
@@ -63,9 +46,6 @@
   </si>
   <si>
     <t>f[cm]</t>
-  </si>
-  <si>
-    <t>Miara[cm]</t>
   </si>
   <si>
     <t>Uc</t>
@@ -90,6 +70,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,14 +236,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -269,23 +248,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -603,298 +583,284 @@
   <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.3984375" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B4" s="8" t="s">
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>19.8</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>60.2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f>C5*D5/(C5+D5)</f>
         <v>14.8995</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f>($E$15-E5)^2</f>
         <v>7.3762750663758481E-2</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="15">
-        <f>I4/SQRT(3)</f>
-        <v>5.7735026918962581E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B6" s="3">
+      <c r="H5" s="5"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>58.5</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" ref="E6:E14" si="0">C6*D6/(C6+D6)</f>
         <v>14.681177976952627</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f t="shared" ref="F6:F14" si="1">($E$15-E6)^2</f>
         <v>2.8377956153835516E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B7" s="3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>56</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>14.682476943346506</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>2.9778773133283111E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B8" s="3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>20</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>54</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>14.594594594594595</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>1.1097172106733105E-3</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B9" s="3">
+      <c r="H8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>20.5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>51.5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>14.663194444444445</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>1.2452028278438052E-3</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B10" s="3">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>20.8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>49</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>14.601719197707737</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>6.8580166243649974E-4</v>
       </c>
-      <c r="H10" s="13">
-        <f>SQRT(F16^2+I5^2)</f>
-        <v>6.8610091092230679E-2</v>
-      </c>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B11" s="3">
+      <c r="H10" s="11">
+        <f>F16</f>
+        <v>3.7067657956105844E-2</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>21.1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>46.6</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>14.523781388478582</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>1.0842145652770103E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B12" s="3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>21.6</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>44</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>14.487804878048783</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>1.9628608178593236E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B13" s="3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
         <v>9</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>22.6</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>41.4</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>14.619375</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>7.2795243439112222E-5</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B14" s="5">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>23.4</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>38.299999999999997</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>14.52544570502431</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>1.0498319603350743E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10">
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7">
         <f>AVERAGE(E5:E14)</f>
         <v>14.62790701285976</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="2">
         <f>SUM(F5:F14)</f>
         <v>0.12366101397157714</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="2" t="s">
+    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="14">
         <f>SQRT(F15/(B14*B13))</f>
         <v>3.7067657956105844E-2</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="17"/>
+      <c r="H16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>